<commit_message>
feat: Afina detección de RUT en OCR y corrige flujo de logout
</commit_message>
<xml_diff>
--- a/participaciones_export.xlsx
+++ b/participaciones_export.xlsx
@@ -124,161 +124,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>15</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>16</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>15</col>
-      <colOff>0</colOff>
-      <row>2</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>16</col>
-      <colOff>0</colOff>
-      <row>2</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>15</col>
-      <colOff>0</colOff>
-      <row>3</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>16</col>
-      <colOff>0</colOff>
-      <row>3</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="1428750"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -568,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,83 +533,93 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Angel Gonzalez</t>
+          <t>Danilo Gonzalez</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>usuario3@ejemplo.com</t>
+          <t>usuario1@ejemplo.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Universo Matucana</t>
+          <t>Geocentro Lira</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0303</t>
+          <t>0101</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>si</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>13.473.719-0</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-09-15T20:25:20.246991</t>
+          <t>2025-09-16T00:26:37.496088</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-09-15T20:24:13.499291</t>
+          <t>2025-09-16T00:26:17.250750</t>
         </is>
       </c>
       <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="n">
-        <v>2</v>
-      </c>
       <c r="M2" t="n">
-        <v>10.473</v>
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/static/uploads/13473719-0_20250915202500_front_orig.jpg</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>/static/uploads/13473719-0_20250915202500_back.jpg</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
         </is>
       </c>
     </row>
     <row r="3" ht="112.5" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13.473.719-0</t>
+          <t>13473719-0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Danilo Gonzalez</t>
+          <t>Angel Gonzalez</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>usuario1@ejemplo.com</t>
+          <t>usuario3@ejemplo.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -774,7 +629,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0101</t>
+          <t>0303</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -784,117 +639,298 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Sí</t>
+          <t>No</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>13.473.719-0</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-09-15T20:23:30.844180</t>
+          <t>2025-09-16T00:17:45.605196</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025-09-15T20:22:47.939829</t>
+          <t>2025-09-16T00:17:16.888342</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>10.526</v>
+        <v>0</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>/static/uploads/13473719-0_20250915202311_front_orig.jpg</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>/static/uploads/13473719-0_20250915202311_back.jpg</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
         </is>
       </c>
     </row>
     <row r="4" ht="112.5" customHeight="1">
       <c r="A4" t="inlineStr">
         <is>
+          <t>13900270-9</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Marcela Díaz</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>usuario2@ejemplo.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Universo Matucana</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0202</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-09-16T02:10:18.123325</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="112.5" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>13.473.719-0</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Danilo Gonzalez</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>usuario1@ejemplo.com</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Universo Matucana</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0101</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-09-16T01:06:26.058975</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025-09-16T01:05:50.734886</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="112.5" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13.473.719-0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Danilo Gonzalez</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>usuario1@ejemplo.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Universo Matucana</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>0404</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>si</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>13.473.719-0</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2025-09-15T20:23:30.844180</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2025-09-15T20:22:47.939829</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-09-16T01:06:26.199369</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025-09-16T01:05:50.734886</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
         <v>1</v>
       </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>10.526</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>/static/uploads/13473719-0_20250915202311_front_orig.jpg</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>/static/uploads/13473719-0_20250915202311_back.jpg</t>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>URL no disponible</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit: Project setup with Flask and Cognito scripts
</commit_message>
<xml_diff>
--- a/participaciones_export.xlsx
+++ b/participaciones_export.xlsx
@@ -124,6 +124,111 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>16</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1428750"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>15</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2286000" cy="1028700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>16</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2286000" cy="1028700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -413,7 +518,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,19 +673,19 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-09-16T00:26:37.496088</t>
+          <t>2025-09-16T03:37:30.356820</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-09-16T00:26:17.250750</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -639,51 +744,41 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>134737190</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-09-16T04:11:22.131582</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2025-09-16T00:17:45.605196</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2025-09-16T00:17:16.888342</t>
         </is>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>/static/uploads/6488e438-5041-7030-84c9-b7c11060a8b5_1757995863.12796_WhatsApp_Image_2023-11-16_at_7.11.34_PM_1.jpeg</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
+          <t>/static/uploads/6488e438-5041-7030-84c9-b7c11060a8b5_1757995863.129084_WhatsApp_Image_2023-11-16_at_7.11.34_PM.jpeg</t>
         </is>
       </c>
     </row>
@@ -720,17 +815,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>139002709</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2025-09-16T02:10:18.123325</t>
+          <t>2025-09-16T04:15:07.274086</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -749,188 +844,17 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>/static/uploads/84c86438-e071-7016-635a-d50a8efcf635_1757996097.401468_17579960117989222010735305516883.jpg</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="112.5" customHeight="1">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>13.473.719-0</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Danilo Gonzalez</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>usuario1@ejemplo.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Universo Matucana</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0101</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2025-09-16T01:06:26.058975</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2025-09-16T01:05:50.734886</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="112.5" customHeight="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>13.473.719-0</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Danilo Gonzalez</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>usuario1@ejemplo.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Universo Matucana</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0404</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2025-09-16T01:06:26.199369</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2025-09-16T01:05:50.734886</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>URL no disponible</t>
+          <t>/static/uploads/84c86438-e071-7016-635a-d50a8efcf635_1757996097.430011_17579960404017116731968949577657.jpg</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>